<commit_message>
Updates to controllers, Mikilua
 - Experimented with VW control - not converging
 - minor changes (with improvements) in VV and storage controls
 - updates to DSS files with smaller PV, accurate voltage bases, etc.
 - updates to controller settings for Mikilua scenarios; also ESS controller settings
</commit_message>
<xml_diff>
--- a/ProjectFiles/Mikilua/PyDSS Settings/HP-VV-VW-B2-CSS30-VV/pyControllerList/PV Controller.xlsx
+++ b/ProjectFiles/Mikilua/PyDSS Settings/HP-VV-VW-B2-CSS30-VV/pyControllerList/PV Controller.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D47705-C109-CC40-94A7-09FF8FC7670A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3007E455-08BE-3349-9986-49BB553681FB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="4880" windowWidth="28080" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2443,6 +2443,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Courier New"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2518,24 +2537,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2942,12 +2943,12 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="uMinC" dataDxfId="8"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="uMaxC" dataDxfId="7"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="PminVW" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="VWtype" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="%PCutin" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="%PCutout" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Efficiency" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="pDampCoef" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="VWtype" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="%PCutin" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="%PCutout" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Efficiency" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Priority" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="pDampCoef" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3218,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y648"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A512" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="A648" sqref="A648"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40162,7 +40163,7 @@
       <c r="X480" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y480" s="4">
+      <c r="Y480" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -40239,7 +40240,7 @@
       <c r="X481" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y481" s="4">
+      <c r="Y481" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -40316,7 +40317,7 @@
       <c r="X482" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y482" s="4">
+      <c r="Y482" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -40393,7 +40394,7 @@
       <c r="X483" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y483" s="4">
+      <c r="Y483" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -40470,7 +40471,7 @@
       <c r="X484" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y484" s="4">
+      <c r="Y484" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -40547,7 +40548,7 @@
       <c r="X485" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y485" s="4">
+      <c r="Y485" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -40624,7 +40625,7 @@
       <c r="X486" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y486" s="4">
+      <c r="Y486" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -40701,7 +40702,7 @@
       <c r="X487" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y487" s="4">
+      <c r="Y487" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -40778,7 +40779,7 @@
       <c r="X488" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y488" s="4">
+      <c r="Y488" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -40855,7 +40856,7 @@
       <c r="X489" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y489" s="4">
+      <c r="Y489" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -40932,7 +40933,7 @@
       <c r="X490" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y490" s="4">
+      <c r="Y490" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -41009,7 +41010,7 @@
       <c r="X491" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y491" s="4">
+      <c r="Y491" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -41086,7 +41087,7 @@
       <c r="X492" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y492" s="4">
+      <c r="Y492" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -41163,7 +41164,7 @@
       <c r="X493" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y493" s="4">
+      <c r="Y493" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -41240,7 +41241,7 @@
       <c r="X494" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y494" s="4">
+      <c r="Y494" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -41317,7 +41318,7 @@
       <c r="X495" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y495" s="4">
+      <c r="Y495" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -41394,7 +41395,7 @@
       <c r="X496" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y496" s="4">
+      <c r="Y496" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -41471,7 +41472,7 @@
       <c r="X497" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y497" s="4">
+      <c r="Y497" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -41548,7 +41549,7 @@
       <c r="X498" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y498" s="4">
+      <c r="Y498" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -41625,7 +41626,7 @@
       <c r="X499" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y499" s="4">
+      <c r="Y499" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -41702,7 +41703,7 @@
       <c r="X500" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y500" s="4">
+      <c r="Y500" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -44320,7 +44321,7 @@
       <c r="X534" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y534" s="25">
+      <c r="Y534" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -44474,7 +44475,7 @@
       <c r="X536" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y536" s="25">
+      <c r="Y536" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -44628,7 +44629,7 @@
       <c r="X538" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y538" s="25">
+      <c r="Y538" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -44782,7 +44783,7 @@
       <c r="X540" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y540" s="25">
+      <c r="Y540" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -44936,7 +44937,7 @@
       <c r="X542" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y542" s="25">
+      <c r="Y542" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45090,7 +45091,7 @@
       <c r="X544" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y544" s="25">
+      <c r="Y544" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45244,7 +45245,7 @@
       <c r="X546" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y546" s="25">
+      <c r="Y546" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45398,7 +45399,7 @@
       <c r="X548" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y548" s="25">
+      <c r="Y548" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45552,7 +45553,7 @@
       <c r="X550" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y550" s="25">
+      <c r="Y550" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45706,7 +45707,7 @@
       <c r="X552" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y552" s="25">
+      <c r="Y552" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -45860,7 +45861,7 @@
       <c r="X554" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y554" s="25">
+      <c r="Y554" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46014,7 +46015,7 @@
       <c r="X556" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y556" s="25">
+      <c r="Y556" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46168,7 +46169,7 @@
       <c r="X558" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y558" s="25">
+      <c r="Y558" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46322,7 +46323,7 @@
       <c r="X560" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y560" s="25">
+      <c r="Y560" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46476,7 +46477,7 @@
       <c r="X562" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y562" s="25">
+      <c r="Y562" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46630,7 +46631,7 @@
       <c r="X564" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y564" s="25">
+      <c r="Y564" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46784,7 +46785,7 @@
       <c r="X566" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y566" s="25">
+      <c r="Y566" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -46938,7 +46939,7 @@
       <c r="X568" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y568" s="25">
+      <c r="Y568" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47092,7 +47093,7 @@
       <c r="X570" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y570" s="25">
+      <c r="Y570" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47246,7 +47247,7 @@
       <c r="X572" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y572" s="25">
+      <c r="Y572" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47400,7 +47401,7 @@
       <c r="X574" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y574" s="25">
+      <c r="Y574" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47554,7 +47555,7 @@
       <c r="X576" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y576" s="25">
+      <c r="Y576" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47708,7 +47709,7 @@
       <c r="X578" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y578" s="25">
+      <c r="Y578" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -47862,7 +47863,7 @@
       <c r="X580" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y580" s="25">
+      <c r="Y580" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48016,7 +48017,7 @@
       <c r="X582" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y582" s="25">
+      <c r="Y582" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48170,7 +48171,7 @@
       <c r="X584" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y584" s="25">
+      <c r="Y584" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48324,7 +48325,7 @@
       <c r="X586" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y586" s="25">
+      <c r="Y586" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48478,7 +48479,7 @@
       <c r="X588" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y588" s="25">
+      <c r="Y588" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48632,7 +48633,7 @@
       <c r="X590" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y590" s="25">
+      <c r="Y590" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48786,7 +48787,7 @@
       <c r="X592" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y592" s="25">
+      <c r="Y592" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -48940,7 +48941,7 @@
       <c r="X594" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y594" s="25">
+      <c r="Y594" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49094,7 +49095,7 @@
       <c r="X596" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y596" s="25">
+      <c r="Y596" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49248,7 +49249,7 @@
       <c r="X598" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y598" s="25">
+      <c r="Y598" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49402,7 +49403,7 @@
       <c r="X600" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y600" s="25">
+      <c r="Y600" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49556,7 +49557,7 @@
       <c r="X602" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y602" s="25">
+      <c r="Y602" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49710,7 +49711,7 @@
       <c r="X604" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y604" s="25">
+      <c r="Y604" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -49864,7 +49865,7 @@
       <c r="X606" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y606" s="25">
+      <c r="Y606" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50018,7 +50019,7 @@
       <c r="X608" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y608" s="25">
+      <c r="Y608" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50172,7 +50173,7 @@
       <c r="X610" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y610" s="25">
+      <c r="Y610" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50326,7 +50327,7 @@
       <c r="X612" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y612" s="25">
+      <c r="Y612" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50480,7 +50481,7 @@
       <c r="X614" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y614" s="25">
+      <c r="Y614" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50634,7 +50635,7 @@
       <c r="X616" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y616" s="25">
+      <c r="Y616" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50788,7 +50789,7 @@
       <c r="X618" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y618" s="25">
+      <c r="Y618" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -50942,7 +50943,7 @@
       <c r="X620" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y620" s="25">
+      <c r="Y620" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51096,7 +51097,7 @@
       <c r="X622" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y622" s="25">
+      <c r="Y622" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51250,7 +51251,7 @@
       <c r="X624" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y624" s="25">
+      <c r="Y624" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51404,7 +51405,7 @@
       <c r="X626" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y626" s="25">
+      <c r="Y626" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51558,7 +51559,7 @@
       <c r="X628" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y628" s="25">
+      <c r="Y628" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51712,7 +51713,7 @@
       <c r="X630" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y630" s="25">
+      <c r="Y630" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -51866,7 +51867,7 @@
       <c r="X632" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y632" s="25">
+      <c r="Y632" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52020,7 +52021,7 @@
       <c r="X634" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y634" s="25">
+      <c r="Y634" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52174,7 +52175,7 @@
       <c r="X636" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y636" s="25">
+      <c r="Y636" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52328,7 +52329,7 @@
       <c r="X638" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y638" s="25">
+      <c r="Y638" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52482,7 +52483,7 @@
       <c r="X640" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y640" s="25">
+      <c r="Y640" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52636,7 +52637,7 @@
       <c r="X642" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y642" s="25">
+      <c r="Y642" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52790,7 +52791,7 @@
       <c r="X644" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y644" s="25">
+      <c r="Y644" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -52944,7 +52945,7 @@
       <c r="X646" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y646" s="25">
+      <c r="Y646" s="26">
         <v>0.7</v>
       </c>
     </row>
@@ -53098,7 +53099,7 @@
       <c r="X648" s="4">
         <v>0.15</v>
       </c>
-      <c r="Y648" s="25">
+      <c r="Y648" s="26">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>